<commit_message>
added cost information into the front end store. also added cost breakdown component and view
</commit_message>
<xml_diff>
--- a/cost breakdown.xlsx
+++ b/cost breakdown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\workspace\java-final-capstone-team7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CB55063-7A5A-4C43-A6E6-40A84CB11748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC3A5493-6F42-444F-9EC9-0528E3CBA463}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F860004D-61CB-4DE1-A5F2-07380193DBA2}"/>
   </bookViews>
@@ -243,37 +243,42 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -588,7 +593,7 @@
   <dimension ref="A1:P61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10:O13"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -596,7 +601,7 @@
     <col min="1" max="1" width="21.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="11.08984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.36328125" customWidth="1"/>
-    <col min="5" max="5" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.90625" customWidth="1"/>
     <col min="6" max="6" width="5.36328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.08984375" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="13.6328125" bestFit="1" customWidth="1"/>
@@ -607,49 +612,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="3" t="s">
+      <c r="E1" s="11"/>
+      <c r="F1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="2" t="s">
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="5"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="4"/>
       <c r="L2" t="s">
         <v>46</v>
       </c>
@@ -667,271 +672,286 @@
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="5">
         <v>10</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <v>26</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <f>AVERAGE(B3:C3)</f>
         <v>18</v>
       </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="6" t="s">
+      <c r="E3" s="14">
+        <f>D3/D$17</f>
+        <v>0.18045112781954886</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="5">
         <v>19900</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="5">
         <v>449000</v>
       </c>
-      <c r="I3" s="6">
+      <c r="I3" s="5">
         <v>134072</v>
       </c>
-      <c r="J3" s="9">
+      <c r="J3" s="7">
         <f>I3/1000</f>
         <v>134.072</v>
       </c>
-      <c r="L3" s="12">
+      <c r="L3" s="8">
         <v>1000</v>
       </c>
-      <c r="M3" s="9">
+      <c r="M3" s="7">
         <f>AVERAGE(I3,I8)</f>
         <v>133000.5</v>
       </c>
-      <c r="N3" s="9">
+      <c r="N3" s="7">
         <f>AVERAGE(I4,I9)</f>
         <v>271914</v>
       </c>
-      <c r="O3" s="9">
+      <c r="O3" s="7">
         <f>AVERAGE(I5,I10)</f>
         <v>381164</v>
       </c>
-      <c r="P3" s="9">
+      <c r="P3" s="7">
         <f>AVERAGE(I6,I11)</f>
         <v>127029</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <v>0.4</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>4</v>
       </c>
-      <c r="D4" s="6">
-        <f t="shared" ref="D4:D19" si="0">AVERAGE(B4:C4)</f>
+      <c r="D4" s="5">
+        <f t="shared" ref="D4:D14" si="0">AVERAGE(B4:C4)</f>
         <v>2.2000000000000002</v>
       </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="6" t="s">
+      <c r="E4" s="14">
+        <f t="shared" ref="E4:E15" si="1">D4/D$17</f>
+        <v>2.2055137844611529E-2</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="5">
         <v>69900</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="5">
         <v>1445000</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="5">
         <v>299676</v>
       </c>
-      <c r="J4" s="9">
-        <f t="shared" ref="J4:J6" si="1">I4/1000</f>
+      <c r="J4" s="7">
+        <f t="shared" ref="J4:J6" si="2">I4/1000</f>
         <v>299.67599999999999</v>
       </c>
-      <c r="L4" s="12">
+      <c r="L4" s="8">
         <v>1500</v>
       </c>
-      <c r="M4" s="9">
+      <c r="M4" s="7">
         <f>AVERAGE(I23,I18)</f>
         <v>132212.5</v>
       </c>
-      <c r="N4" s="9">
+      <c r="N4" s="7">
         <f>AVERAGE(I24,I19)</f>
         <v>308454.5</v>
       </c>
-      <c r="O4" s="9">
+      <c r="O4" s="7">
         <f>AVERAGE(I25,I20)</f>
         <v>411185.5</v>
       </c>
-      <c r="P4" s="9">
+      <c r="P4" s="7">
         <f>AVERAGE(I26,I21)</f>
         <v>149176</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>1.5</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>2.5</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="6" t="s">
+      <c r="E5" s="14">
+        <f t="shared" si="1"/>
+        <v>2.0050125313283207E-2</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="5">
         <v>49000</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="5">
         <v>725000</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="5">
         <v>330740</v>
       </c>
-      <c r="J5" s="9">
-        <f t="shared" si="1"/>
+      <c r="J5" s="7">
+        <f t="shared" si="2"/>
         <v>330.74</v>
       </c>
-      <c r="L5" s="12">
+      <c r="L5" s="8">
         <v>2000</v>
       </c>
-      <c r="M5" s="9">
+      <c r="M5" s="7">
         <f>AVERAGE(I33,I38)</f>
         <v>144626.5</v>
       </c>
-      <c r="N5" s="9">
+      <c r="N5" s="7">
         <f>AVERAGE(I34,I39)</f>
         <v>363193.5</v>
       </c>
-      <c r="O5" s="9">
+      <c r="O5" s="7">
         <f>AVERAGE(I35,I40)</f>
         <v>478452</v>
       </c>
-      <c r="P5" s="9">
+      <c r="P5" s="7">
         <f>AVERAGE(I36,I41)</f>
         <v>186817</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>1</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>5</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="8" t="s">
+      <c r="E6" s="14">
+        <f t="shared" si="1"/>
+        <v>3.007518796992481E-2</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="6">
         <v>22000</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="6">
         <v>329900</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I6" s="6">
         <v>130497</v>
       </c>
-      <c r="J6" s="9">
-        <f t="shared" si="1"/>
+      <c r="J6" s="7">
+        <f t="shared" si="2"/>
         <v>130.49700000000001</v>
       </c>
-      <c r="L6" s="12">
+      <c r="L6" s="8">
         <v>2500</v>
       </c>
-      <c r="M6" s="9">
+      <c r="M6" s="7">
         <f>AVERAGE(I48,I53)</f>
         <v>173637.5</v>
       </c>
-      <c r="N6" s="9">
+      <c r="N6" s="7">
         <f>AVERAGE(I59,I54)</f>
         <v>238284.5</v>
       </c>
-      <c r="O6" s="9">
+      <c r="O6" s="7">
         <f>AVERAGE(I55,I50)</f>
         <v>568719</v>
       </c>
-      <c r="P6" s="9">
+      <c r="P6" s="7">
         <f>AVERAGE(I56,I51)</f>
         <v>241237</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="5">
         <v>2</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>15</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <f t="shared" si="0"/>
         <v>8.5</v>
       </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="7" t="s">
+      <c r="E7" s="14">
+        <f t="shared" si="1"/>
+        <v>8.5213032581453629E-2</v>
+      </c>
+      <c r="F7" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
       <c r="L7" t="s">
         <v>48</v>
       </c>
-      <c r="M7" s="9">
+      <c r="M7" s="7">
         <f>AVERAGE(M3:M6)</f>
         <v>145869.25</v>
       </c>
-      <c r="N7" s="9">
-        <f t="shared" ref="N7:P7" si="2">AVERAGE(N3:N6)</f>
+      <c r="N7" s="7">
+        <f t="shared" ref="N7:P7" si="3">AVERAGE(N3:N6)</f>
         <v>295461.625</v>
       </c>
-      <c r="O7" s="9">
-        <f t="shared" si="2"/>
+      <c r="O7" s="7">
+        <f t="shared" si="3"/>
         <v>459880.125</v>
       </c>
-      <c r="P7" s="9">
-        <f t="shared" si="2"/>
+      <c r="P7" s="7">
+        <f t="shared" si="3"/>
         <v>176064.75</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="6" t="s">
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="6">
         <v>29000</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="6">
         <v>439900</v>
       </c>
-      <c r="I8" s="8">
+      <c r="I8" s="6">
         <v>131929</v>
       </c>
-      <c r="J8" s="9">
+      <c r="J8" s="7">
         <f>I8/1000</f>
         <v>131.929</v>
       </c>
@@ -940,34 +960,37 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="5">
         <v>1.6</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>17.2</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <f t="shared" si="0"/>
         <v>9.4</v>
       </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="6" t="s">
+      <c r="E9" s="14">
+        <f t="shared" si="1"/>
+        <v>9.4235588972431075E-2</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="5">
         <v>43000</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="5">
         <v>487000</v>
       </c>
-      <c r="I9" s="6">
+      <c r="I9" s="5">
         <v>244152</v>
       </c>
-      <c r="J9" s="9">
-        <f t="shared" ref="J9:J11" si="3">I9/1000</f>
+      <c r="J9" s="7">
+        <f t="shared" ref="J9:J11" si="4">I9/1000</f>
         <v>244.15199999999999</v>
       </c>
       <c r="K9" s="1"/>
@@ -985,246 +1008,264 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="5">
         <v>2</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="5">
         <v>4</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="5">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="6" t="s">
+      <c r="E10" s="14">
+        <f t="shared" si="1"/>
+        <v>3.007518796992481E-2</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="5">
         <v>119995</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="5">
         <v>3800000</v>
       </c>
-      <c r="I10" s="6">
+      <c r="I10" s="5">
         <v>431588</v>
       </c>
-      <c r="J10" s="9">
-        <f t="shared" si="3"/>
+      <c r="J10" s="7">
+        <f t="shared" si="4"/>
         <v>431.58800000000002</v>
       </c>
       <c r="L10" t="s">
         <v>23</v>
       </c>
-      <c r="M10" s="9">
+      <c r="M10" s="7">
         <f>AVERAGE(J8,J3,J18,J23,J33,J38,J48,J53)</f>
         <v>90.727604166666652</v>
       </c>
-      <c r="N10" s="9">
+      <c r="N10" s="7">
         <f>AVERAGE(J13,J28,J43,J58)</f>
         <v>22.665500000000002</v>
       </c>
-      <c r="O10" s="13">
+      <c r="O10" s="9">
         <v>0.72</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="5">
         <v>2</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="5">
         <v>4</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="5">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="8" t="s">
+      <c r="E11" s="14">
+        <f t="shared" si="1"/>
+        <v>3.007518796992481E-2</v>
+      </c>
+      <c r="F11" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="6">
         <v>29000</v>
       </c>
-      <c r="H11" s="8">
+      <c r="H11" s="6">
         <v>299900</v>
       </c>
-      <c r="I11" s="8">
+      <c r="I11" s="6">
         <v>123561</v>
       </c>
-      <c r="J11" s="9">
-        <f t="shared" si="3"/>
+      <c r="J11" s="7">
+        <f t="shared" si="4"/>
         <v>123.56100000000001</v>
       </c>
       <c r="L11" t="s">
         <v>24</v>
       </c>
-      <c r="M11" s="9">
+      <c r="M11" s="7">
         <f>AVERAGE(J49,J39,J34, J4,J9,J19,J24,J54)</f>
         <v>207.14372083333336</v>
       </c>
-      <c r="N11" s="9">
+      <c r="N11" s="7">
         <f>AVERAGE(J14,J29,J44,J59)</f>
         <v>48.901666666666671</v>
       </c>
-      <c r="O11" s="13">
+      <c r="O11" s="9">
         <v>1.66</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="5">
         <v>1.5</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="5">
         <v>3</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="5">
         <f t="shared" si="0"/>
         <v>2.25</v>
       </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="7" t="s">
+      <c r="E12" s="14">
+        <f t="shared" si="1"/>
+        <v>2.2556390977443608E-2</v>
+      </c>
+      <c r="F12" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
       <c r="L12" t="s">
         <v>25</v>
       </c>
-      <c r="M12" s="9">
+      <c r="M12" s="7">
         <f>AVERAGE(J20,J25,J35,J40,J50,J55)</f>
         <v>246.94575555555551</v>
       </c>
-      <c r="N12" s="9">
+      <c r="N12" s="7">
         <f>AVERAGE(J15,J30,J45,J60)</f>
         <v>62.662437499999996</v>
       </c>
-      <c r="O12" s="13">
+      <c r="O12" s="9">
         <v>1.98</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="5">
         <v>1.6</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="5">
         <v>5.2</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="5">
         <f t="shared" si="0"/>
         <v>3.4000000000000004</v>
       </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="6" t="s">
+      <c r="E13" s="14">
+        <f t="shared" si="1"/>
+        <v>3.4085213032581455E-2</v>
+      </c>
+      <c r="F13" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" s="6">
         <v>5000</v>
       </c>
-      <c r="H13" s="8">
+      <c r="H13" s="6">
         <v>599900</v>
       </c>
-      <c r="I13" s="8">
+      <c r="I13" s="6">
         <v>83688</v>
       </c>
-      <c r="J13" s="9">
+      <c r="J13" s="7">
         <f>I13/2000</f>
         <v>41.844000000000001</v>
       </c>
       <c r="L13" t="s">
         <v>26</v>
       </c>
-      <c r="M13" s="9">
+      <c r="M13" s="7">
         <f>AVERAGE(J6,J11,J21,J26,J36,J41,J51,J56)</f>
         <v>104.09574166666667</v>
       </c>
-      <c r="N13" s="9">
+      <c r="N13" s="7">
         <f>AVERAGE(J16,J31,J46,J61)</f>
         <v>20.329020833333335</v>
       </c>
-      <c r="O13" s="13">
+      <c r="O13" s="9">
         <v>0.84</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="5">
         <v>10</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="5">
         <v>20</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="5">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="E14" s="9"/>
-      <c r="F14" s="6" t="s">
+      <c r="E14" s="14">
+        <f t="shared" si="1"/>
+        <v>0.15037593984962405</v>
+      </c>
+      <c r="F14" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="8">
+      <c r="G14" s="6">
         <v>3000</v>
       </c>
-      <c r="H14" s="8">
+      <c r="H14" s="6">
         <v>2750000</v>
       </c>
-      <c r="I14" s="8">
+      <c r="I14" s="6">
         <v>180560</v>
       </c>
-      <c r="J14" s="9">
-        <f t="shared" ref="J14:J16" si="4">I14/2000</f>
+      <c r="J14" s="7">
+        <f t="shared" ref="J14:J16" si="5">I14/2000</f>
         <v>90.28</v>
       </c>
       <c r="L14" t="s">
         <v>43</v>
       </c>
-      <c r="M14" s="9">
+      <c r="M14" s="7">
         <f>AVERAGE(M10:M13)</f>
         <v>162.22820555555555</v>
       </c>
-      <c r="N14" s="9">
+      <c r="N14" s="7">
         <f>AVERAGE(N10:N13)</f>
         <v>38.639656250000002</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="6">
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="5">
         <v>30</v>
       </c>
-      <c r="E15" s="9"/>
-      <c r="F15" s="6" t="s">
+      <c r="E15" s="14">
+        <f t="shared" si="1"/>
+        <v>0.3007518796992481</v>
+      </c>
+      <c r="F15" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G15" s="8">
+      <c r="G15" s="6">
         <v>15000</v>
       </c>
-      <c r="H15" s="8">
+      <c r="H15" s="6">
         <v>1500000</v>
       </c>
-      <c r="I15" s="8">
+      <c r="I15" s="6">
         <v>231369</v>
       </c>
-      <c r="J15" s="9">
-        <f t="shared" si="4"/>
+      <c r="J15" s="7">
+        <f t="shared" si="5"/>
         <v>115.6845</v>
       </c>
       <c r="L15" t="s">
@@ -1240,23 +1281,24 @@
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A16" s="11"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="F16" s="8" t="s">
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G16" s="6">
         <v>6000</v>
       </c>
-      <c r="H16" s="8">
+      <c r="H16" s="6">
         <v>395000</v>
       </c>
-      <c r="I16" s="8">
+      <c r="I16" s="6">
         <v>75061</v>
       </c>
-      <c r="J16" s="9">
-        <f t="shared" si="4"/>
+      <c r="J16" s="7">
+        <f t="shared" si="5"/>
         <v>37.530500000000004</v>
       </c>
     </row>
@@ -1264,791 +1306,792 @@
       <c r="C17" t="s">
         <v>47</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D17" s="16">
         <f>SUM(D3:D15)</f>
         <v>99.75</v>
       </c>
-      <c r="E17" s="9"/>
-      <c r="F17" s="7" t="s">
+      <c r="E17" s="7"/>
+      <c r="F17" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G18" s="8">
+      <c r="G18" s="6">
         <v>19900</v>
       </c>
-      <c r="H18" s="8">
+      <c r="H18" s="6">
         <v>449000</v>
       </c>
-      <c r="I18" s="8">
+      <c r="I18" s="6">
         <v>132158</v>
       </c>
-      <c r="J18" s="9">
+      <c r="J18" s="7">
         <f>I18/1500</f>
         <v>88.105333333333334</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="F19" s="6" t="s">
+      <c r="F19" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G19" s="6">
+      <c r="G19" s="5">
         <v>69900</v>
       </c>
-      <c r="H19" s="6">
+      <c r="H19" s="5">
         <v>1445000</v>
       </c>
-      <c r="I19" s="6">
+      <c r="I19" s="5">
         <v>367519</v>
       </c>
-      <c r="J19" s="9">
-        <f t="shared" ref="J19:J21" si="5">I19/1500</f>
+      <c r="J19" s="7">
+        <f t="shared" ref="J19:J21" si="6">I19/1500</f>
         <v>245.01266666666666</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G20" s="6">
+      <c r="G20" s="5">
         <v>169000</v>
       </c>
-      <c r="H20" s="6">
+      <c r="H20" s="5">
         <v>725000</v>
       </c>
-      <c r="I20" s="6">
+      <c r="I20" s="5">
         <v>371462</v>
       </c>
-      <c r="J20" s="9">
-        <f t="shared" si="5"/>
+      <c r="J20" s="7">
+        <f t="shared" si="6"/>
         <v>247.64133333333334</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="6"/>
-      <c r="F21" s="8" t="s">
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="5"/>
+      <c r="F21" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G21" s="8">
+      <c r="G21" s="6">
         <v>29000</v>
       </c>
-      <c r="H21" s="8">
+      <c r="H21" s="6">
         <v>385000</v>
       </c>
-      <c r="I21" s="8">
+      <c r="I21" s="6">
         <v>173669</v>
       </c>
-      <c r="J21" s="9">
-        <f t="shared" si="5"/>
+      <c r="J21" s="7">
+        <f t="shared" si="6"/>
         <v>115.77933333333333</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="5">
         <v>36750</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C22" s="5">
         <v>66500</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D22" s="5">
         <f>AVERAGE(B22:C22)</f>
         <v>51625</v>
       </c>
-      <c r="F22" s="7" t="s">
+      <c r="F22" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="6">
+      <c r="B23" s="5">
         <v>6</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C23" s="5">
         <v>20</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23" s="5">
         <f>AVERAGE(B23:C23)</f>
         <v>13</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="F23" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G23" s="8">
+      <c r="G23" s="6">
         <v>29000</v>
       </c>
-      <c r="H23" s="8">
+      <c r="H23" s="6">
         <v>439900</v>
       </c>
-      <c r="I23" s="8">
+      <c r="I23" s="6">
         <v>132267</v>
       </c>
-      <c r="J23" s="9">
+      <c r="J23" s="7">
         <f>I23/1500</f>
         <v>88.177999999999997</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B24" s="5">
         <v>10000</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C24" s="5">
         <v>30000</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D24" s="5">
         <f>AVERAGE(B24:C24)</f>
         <v>20000</v>
       </c>
       <c r="E24" s="1"/>
-      <c r="F24" s="6" t="s">
+      <c r="F24" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G24" s="6">
+      <c r="G24" s="5">
         <v>43000</v>
       </c>
-      <c r="H24" s="6">
+      <c r="H24" s="5">
         <v>487000</v>
       </c>
-      <c r="I24" s="6">
+      <c r="I24" s="5">
         <v>249390</v>
       </c>
-      <c r="J24" s="9">
-        <f t="shared" ref="J24:J26" si="6">I24/1500</f>
+      <c r="J24" s="7">
+        <f t="shared" ref="J24:J26" si="7">I24/1500</f>
         <v>166.26</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="6">
+      <c r="B25" s="5">
         <v>4000</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C25" s="5">
         <v>11250</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25" s="5">
         <f>AVERAGE(B25:C25)</f>
         <v>7625</v>
       </c>
-      <c r="F25" s="6" t="s">
+      <c r="F25" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G25" s="6">
+      <c r="G25" s="5">
         <v>119995</v>
       </c>
-      <c r="H25" s="6">
+      <c r="H25" s="5">
         <v>3800000</v>
       </c>
-      <c r="I25" s="6">
+      <c r="I25" s="5">
         <v>450909</v>
       </c>
-      <c r="J25" s="9">
-        <f t="shared" si="6"/>
+      <c r="J25" s="7">
+        <f t="shared" si="7"/>
         <v>300.60599999999999</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="F26" s="8" t="s">
+      <c r="F26" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G26" s="8">
+      <c r="G26" s="6">
         <v>29000</v>
       </c>
-      <c r="H26" s="8">
+      <c r="H26" s="6">
         <v>299900</v>
       </c>
-      <c r="I26" s="8">
+      <c r="I26" s="6">
         <v>124683</v>
       </c>
-      <c r="J26" s="9">
-        <f t="shared" si="6"/>
+      <c r="J26" s="7">
+        <f t="shared" si="7"/>
         <v>83.122</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="F27" s="7" t="s">
+      <c r="F27" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="F28" s="6" t="s">
+      <c r="F28" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G28" s="8">
+      <c r="G28" s="6">
         <v>5000</v>
       </c>
-      <c r="H28" s="8">
+      <c r="H28" s="6">
         <v>599900</v>
       </c>
-      <c r="I28" s="8">
+      <c r="I28" s="6">
         <v>83688</v>
       </c>
-      <c r="J28" s="9">
+      <c r="J28" s="7">
         <f>I28/4000</f>
         <v>20.922000000000001</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="F29" s="6" t="s">
+      <c r="F29" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G29" s="6">
+      <c r="G29" s="5">
         <v>3000</v>
       </c>
-      <c r="H29" s="6">
+      <c r="H29" s="5">
         <v>2750000</v>
       </c>
-      <c r="I29" s="6">
+      <c r="I29" s="5">
         <v>180560</v>
       </c>
-      <c r="J29" s="9">
-        <f t="shared" ref="J29:J31" si="7">I29/4000</f>
+      <c r="J29" s="7">
+        <f t="shared" ref="J29:J31" si="8">I29/4000</f>
         <v>45.14</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="F30" s="6" t="s">
+      <c r="F30" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G30" s="6">
+      <c r="G30" s="5">
         <v>15000</v>
       </c>
-      <c r="H30" s="6">
+      <c r="H30" s="5">
         <v>1500000</v>
       </c>
-      <c r="I30" s="6">
+      <c r="I30" s="5">
         <v>231369</v>
       </c>
-      <c r="J30" s="9">
-        <f t="shared" si="7"/>
+      <c r="J30" s="7">
+        <f t="shared" si="8"/>
         <v>57.84225</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="F31" s="8" t="s">
+      <c r="F31" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G31" s="8">
+      <c r="G31" s="6">
         <v>6000</v>
       </c>
-      <c r="H31" s="8">
+      <c r="H31" s="6">
         <v>395000</v>
       </c>
-      <c r="I31" s="8">
+      <c r="I31" s="6">
         <v>75061</v>
       </c>
-      <c r="J31" s="9">
-        <f t="shared" si="7"/>
+      <c r="J31" s="7">
+        <f t="shared" si="8"/>
         <v>18.765250000000002</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="F32" s="7" t="s">
+      <c r="F32" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="7"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
     </row>
     <row r="33" spans="6:10" x14ac:dyDescent="0.35">
-      <c r="F33" s="6" t="s">
+      <c r="F33" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G33" s="8">
+      <c r="G33" s="6">
         <v>30000</v>
       </c>
-      <c r="H33" s="8">
+      <c r="H33" s="6">
         <v>449000</v>
       </c>
-      <c r="I33" s="8">
+      <c r="I33" s="6">
         <v>141820</v>
       </c>
-      <c r="J33" s="9">
+      <c r="J33" s="7">
         <f>I33/2000</f>
         <v>70.91</v>
       </c>
     </row>
     <row r="34" spans="6:10" x14ac:dyDescent="0.35">
-      <c r="F34" s="6" t="s">
+      <c r="F34" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G34" s="8">
+      <c r="G34" s="6">
         <v>59900</v>
       </c>
-      <c r="H34" s="8">
+      <c r="H34" s="6">
         <v>1500000</v>
       </c>
-      <c r="I34" s="8">
+      <c r="I34" s="6">
         <v>454217</v>
       </c>
-      <c r="J34" s="9">
-        <f t="shared" ref="J34:J36" si="8">I34/2000</f>
+      <c r="J34" s="7">
+        <f t="shared" ref="J34:J36" si="9">I34/2000</f>
         <v>227.10849999999999</v>
       </c>
     </row>
     <row r="35" spans="6:10" x14ac:dyDescent="0.35">
-      <c r="F35" s="6" t="s">
+      <c r="F35" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G35" s="8">
+      <c r="G35" s="6">
         <v>249900</v>
       </c>
-      <c r="H35" s="8">
+      <c r="H35" s="6">
         <v>985000</v>
       </c>
-      <c r="I35" s="8">
+      <c r="I35" s="6">
         <v>453014</v>
       </c>
-      <c r="J35" s="9">
-        <f t="shared" si="8"/>
+      <c r="J35" s="7">
+        <f t="shared" si="9"/>
         <v>226.50700000000001</v>
       </c>
     </row>
     <row r="36" spans="6:10" x14ac:dyDescent="0.35">
-      <c r="F36" s="8" t="s">
+      <c r="F36" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G36" s="8">
+      <c r="G36" s="6">
         <v>65000</v>
       </c>
-      <c r="H36" s="8">
+      <c r="H36" s="6">
         <v>469500</v>
       </c>
-      <c r="I36" s="8">
+      <c r="I36" s="6">
         <v>229144</v>
       </c>
-      <c r="J36" s="9">
-        <f t="shared" si="8"/>
+      <c r="J36" s="7">
+        <f t="shared" si="9"/>
         <v>114.572</v>
       </c>
     </row>
     <row r="37" spans="6:10" x14ac:dyDescent="0.35">
-      <c r="F37" s="7" t="s">
+      <c r="F37" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="G37" s="7"/>
-      <c r="H37" s="7"/>
-      <c r="I37" s="7"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10"/>
+      <c r="I37" s="10"/>
     </row>
     <row r="38" spans="6:10" x14ac:dyDescent="0.35">
-      <c r="F38" s="6" t="s">
+      <c r="F38" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G38" s="6">
+      <c r="G38" s="5">
         <v>52000</v>
       </c>
-      <c r="H38" s="6">
+      <c r="H38" s="5">
         <v>439900</v>
       </c>
-      <c r="I38" s="6">
+      <c r="I38" s="5">
         <v>147433</v>
       </c>
-      <c r="J38" s="9">
+      <c r="J38" s="7">
         <f>I38/2000</f>
         <v>73.716499999999996</v>
       </c>
     </row>
     <row r="39" spans="6:10" x14ac:dyDescent="0.35">
-      <c r="F39" s="6" t="s">
+      <c r="F39" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G39" s="6">
+      <c r="G39" s="5">
         <v>67000</v>
       </c>
-      <c r="H39" s="6">
+      <c r="H39" s="5">
         <v>850000</v>
       </c>
-      <c r="I39" s="6">
+      <c r="I39" s="5">
         <v>272170</v>
       </c>
-      <c r="J39" s="9">
-        <f t="shared" ref="J39:J41" si="9">I39/2000</f>
+      <c r="J39" s="7">
+        <f t="shared" ref="J39:J41" si="10">I39/2000</f>
         <v>136.08500000000001</v>
       </c>
     </row>
     <row r="40" spans="6:10" x14ac:dyDescent="0.35">
-      <c r="F40" s="6" t="s">
+      <c r="F40" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G40" s="6">
+      <c r="G40" s="5">
         <v>119995</v>
       </c>
-      <c r="H40" s="6">
+      <c r="H40" s="5">
         <v>3800000</v>
       </c>
-      <c r="I40" s="6">
+      <c r="I40" s="5">
         <v>503890</v>
       </c>
-      <c r="J40" s="9">
-        <f t="shared" si="9"/>
+      <c r="J40" s="7">
+        <f t="shared" si="10"/>
         <v>251.94499999999999</v>
       </c>
     </row>
     <row r="41" spans="6:10" x14ac:dyDescent="0.35">
-      <c r="F41" s="8" t="s">
+      <c r="F41" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G41" s="8">
+      <c r="G41" s="6">
         <v>29000</v>
       </c>
-      <c r="H41" s="8">
+      <c r="H41" s="6">
         <v>630000</v>
       </c>
-      <c r="I41" s="8">
+      <c r="I41" s="6">
         <v>144490</v>
       </c>
-      <c r="J41" s="9">
-        <f t="shared" si="9"/>
+      <c r="J41" s="7">
+        <f t="shared" si="10"/>
         <v>72.245000000000005</v>
       </c>
     </row>
     <row r="42" spans="6:10" x14ac:dyDescent="0.35">
-      <c r="F42" s="7" t="s">
+      <c r="F42" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="G42" s="7"/>
-      <c r="H42" s="7"/>
-      <c r="I42" s="7"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="10"/>
+      <c r="I42" s="10"/>
     </row>
     <row r="43" spans="6:10" x14ac:dyDescent="0.35">
-      <c r="F43" s="6" t="s">
+      <c r="F43" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G43" s="6">
+      <c r="G43" s="5">
         <v>5000</v>
       </c>
-      <c r="H43" s="6">
+      <c r="H43" s="5">
         <v>599900</v>
       </c>
-      <c r="I43" s="6">
+      <c r="I43" s="5">
         <v>83688</v>
       </c>
-      <c r="J43" s="9">
+      <c r="J43" s="7">
         <f>I43/5000</f>
         <v>16.7376</v>
       </c>
     </row>
     <row r="44" spans="6:10" x14ac:dyDescent="0.35">
-      <c r="F44" s="6" t="s">
+      <c r="F44" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G44" s="6">
+      <c r="G44" s="5">
         <v>3000</v>
       </c>
-      <c r="H44" s="6">
+      <c r="H44" s="5">
         <v>2750000</v>
       </c>
-      <c r="I44" s="6">
+      <c r="I44" s="5">
         <v>180560</v>
       </c>
-      <c r="J44" s="9">
-        <f t="shared" ref="J44:J46" si="10">I44/5000</f>
+      <c r="J44" s="7">
+        <f t="shared" ref="J44:J46" si="11">I44/5000</f>
         <v>36.112000000000002</v>
       </c>
     </row>
     <row r="45" spans="6:10" x14ac:dyDescent="0.35">
-      <c r="F45" s="6" t="s">
+      <c r="F45" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G45" s="6">
+      <c r="G45" s="5">
         <v>15000</v>
       </c>
-      <c r="H45" s="6">
+      <c r="H45" s="5">
         <v>1500000</v>
       </c>
-      <c r="I45" s="6">
+      <c r="I45" s="5">
         <v>231369</v>
       </c>
-      <c r="J45" s="9">
-        <f t="shared" si="10"/>
+      <c r="J45" s="7">
+        <f t="shared" si="11"/>
         <v>46.273800000000001</v>
       </c>
     </row>
     <row r="46" spans="6:10" x14ac:dyDescent="0.35">
-      <c r="F46" s="8" t="s">
+      <c r="F46" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G46" s="8">
+      <c r="G46" s="6">
         <v>6000</v>
       </c>
-      <c r="H46" s="8">
+      <c r="H46" s="6">
         <v>395000</v>
       </c>
-      <c r="I46" s="8">
+      <c r="I46" s="6">
         <v>75061</v>
       </c>
-      <c r="J46" s="9">
-        <f t="shared" si="10"/>
+      <c r="J46" s="7">
+        <f t="shared" si="11"/>
         <v>15.0122</v>
       </c>
     </row>
     <row r="47" spans="6:10" x14ac:dyDescent="0.35">
-      <c r="F47" s="7" t="s">
+      <c r="F47" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G47" s="7"/>
-      <c r="H47" s="7"/>
-      <c r="I47" s="7"/>
+      <c r="G47" s="10"/>
+      <c r="H47" s="10"/>
+      <c r="I47" s="10"/>
     </row>
     <row r="48" spans="6:10" x14ac:dyDescent="0.35">
-      <c r="F48" s="6" t="s">
+      <c r="F48" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G48" s="8">
+      <c r="G48" s="6">
         <v>30000</v>
       </c>
-      <c r="H48" s="8">
+      <c r="H48" s="6">
         <v>824900</v>
       </c>
-      <c r="I48" s="8">
+      <c r="I48" s="6">
         <v>194839</v>
       </c>
-      <c r="J48" s="9">
+      <c r="J48" s="7">
         <f>I48/2500</f>
         <v>77.935599999999994</v>
       </c>
     </row>
     <row r="49" spans="6:10" x14ac:dyDescent="0.35">
-      <c r="F49" s="6" t="s">
+      <c r="F49" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G49" s="6">
+      <c r="G49" s="5">
         <v>34000</v>
       </c>
-      <c r="H49" s="6">
+      <c r="H49" s="5">
         <v>1599000</v>
       </c>
-      <c r="I49" s="6">
+      <c r="I49" s="5">
         <v>551130</v>
       </c>
-      <c r="J49" s="9">
-        <f t="shared" ref="J49:J51" si="11">I49/2500</f>
+      <c r="J49" s="7">
+        <f t="shared" ref="J49:J51" si="12">I49/2500</f>
         <v>220.452</v>
       </c>
     </row>
     <row r="50" spans="6:10" x14ac:dyDescent="0.35">
-      <c r="F50" s="6" t="s">
+      <c r="F50" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G50" s="6">
+      <c r="G50" s="5">
         <v>220000</v>
       </c>
-      <c r="H50" s="6">
+      <c r="H50" s="5">
         <v>1485000</v>
       </c>
-      <c r="I50" s="6">
+      <c r="I50" s="5">
         <v>563033</v>
       </c>
-      <c r="J50" s="9">
-        <f t="shared" si="11"/>
+      <c r="J50" s="7">
+        <f t="shared" si="12"/>
         <v>225.2132</v>
       </c>
     </row>
     <row r="51" spans="6:10" x14ac:dyDescent="0.35">
-      <c r="F51" s="8" t="s">
+      <c r="F51" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G51" s="6">
+      <c r="G51" s="5">
         <v>89900</v>
       </c>
-      <c r="H51" s="6">
+      <c r="H51" s="5">
         <v>845000</v>
       </c>
-      <c r="I51" s="6">
+      <c r="I51" s="5">
         <v>303491</v>
       </c>
-      <c r="J51" s="9">
-        <f t="shared" si="11"/>
+      <c r="J51" s="7">
+        <f t="shared" si="12"/>
         <v>121.3964</v>
       </c>
     </row>
     <row r="52" spans="6:10" x14ac:dyDescent="0.35">
-      <c r="F52" s="7" t="s">
+      <c r="F52" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="G52" s="7"/>
-      <c r="H52" s="7"/>
-      <c r="I52" s="7"/>
+      <c r="G52" s="10"/>
+      <c r="H52" s="10"/>
+      <c r="I52" s="10"/>
     </row>
     <row r="53" spans="6:10" x14ac:dyDescent="0.35">
-      <c r="F53" s="6" t="s">
+      <c r="F53" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G53" s="8">
+      <c r="G53" s="6">
         <v>22000</v>
       </c>
-      <c r="H53" s="8">
+      <c r="H53" s="6">
         <v>439900</v>
       </c>
-      <c r="I53" s="8">
+      <c r="I53" s="6">
         <v>152436</v>
       </c>
-      <c r="J53" s="9">
+      <c r="J53" s="7">
         <f>I53/2500</f>
         <v>60.974400000000003</v>
       </c>
     </row>
     <row r="54" spans="6:10" x14ac:dyDescent="0.35">
-      <c r="F54" s="6" t="s">
+      <c r="F54" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G54" s="6">
+      <c r="G54" s="5">
         <v>67000</v>
       </c>
-      <c r="H54" s="6">
+      <c r="H54" s="5">
         <v>850000</v>
       </c>
-      <c r="I54" s="6">
+      <c r="I54" s="5">
         <v>296009</v>
       </c>
-      <c r="J54" s="9">
-        <f t="shared" ref="J54:J56" si="12">I54/2500</f>
+      <c r="J54" s="7">
+        <f t="shared" ref="J54:J56" si="13">I54/2500</f>
         <v>118.4036</v>
       </c>
     </row>
     <row r="55" spans="6:10" x14ac:dyDescent="0.35">
-      <c r="F55" s="6" t="s">
+      <c r="F55" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G55" s="6">
+      <c r="G55" s="5">
         <v>175000</v>
       </c>
-      <c r="H55" s="6">
+      <c r="H55" s="5">
         <v>3800000</v>
       </c>
-      <c r="I55" s="6">
+      <c r="I55" s="5">
         <v>574405</v>
       </c>
-      <c r="J55" s="9">
-        <f t="shared" si="12"/>
+      <c r="J55" s="7">
+        <f t="shared" si="13"/>
         <v>229.762</v>
       </c>
     </row>
     <row r="56" spans="6:10" x14ac:dyDescent="0.35">
-      <c r="F56" s="8" t="s">
+      <c r="F56" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G56" s="8">
+      <c r="G56" s="6">
         <v>14900</v>
       </c>
-      <c r="H56" s="8">
+      <c r="H56" s="6">
         <v>630000</v>
       </c>
-      <c r="I56" s="8">
+      <c r="I56" s="6">
         <v>178983</v>
       </c>
-      <c r="J56" s="9">
-        <f t="shared" si="12"/>
+      <c r="J56" s="7">
+        <f t="shared" si="13"/>
         <v>71.593199999999996</v>
       </c>
     </row>
     <row r="57" spans="6:10" x14ac:dyDescent="0.35">
-      <c r="F57" s="7" t="s">
+      <c r="F57" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="G57" s="7"/>
-      <c r="H57" s="7"/>
-      <c r="I57" s="7"/>
+      <c r="G57" s="10"/>
+      <c r="H57" s="10"/>
+      <c r="I57" s="10"/>
     </row>
     <row r="58" spans="6:10" x14ac:dyDescent="0.35">
-      <c r="F58" s="6" t="s">
+      <c r="F58" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G58" s="6">
+      <c r="G58" s="5">
         <v>5000</v>
       </c>
-      <c r="H58" s="6">
+      <c r="H58" s="5">
         <v>599900</v>
       </c>
-      <c r="I58" s="6">
+      <c r="I58" s="5">
         <v>83688</v>
       </c>
-      <c r="J58" s="9">
+      <c r="J58" s="7">
         <f>I58/7500</f>
         <v>11.1584</v>
       </c>
     </row>
     <row r="59" spans="6:10" x14ac:dyDescent="0.35">
-      <c r="F59" s="6" t="s">
+      <c r="F59" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G59" s="6">
+      <c r="G59" s="5">
         <v>3000</v>
       </c>
-      <c r="H59" s="6">
+      <c r="H59" s="5">
         <v>2750000</v>
       </c>
-      <c r="I59" s="6">
+      <c r="I59" s="5">
         <v>180560</v>
       </c>
-      <c r="J59" s="9">
-        <f t="shared" ref="J59:J61" si="13">I59/7500</f>
+      <c r="J59" s="7">
+        <f t="shared" ref="J59:J61" si="14">I59/7500</f>
         <v>24.074666666666666</v>
       </c>
     </row>
     <row r="60" spans="6:10" x14ac:dyDescent="0.35">
-      <c r="F60" s="6" t="s">
+      <c r="F60" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G60" s="6">
+      <c r="G60" s="5">
         <v>15000</v>
       </c>
-      <c r="H60" s="6">
+      <c r="H60" s="5">
         <v>1500000</v>
       </c>
-      <c r="I60" s="6">
+      <c r="I60" s="5">
         <v>231369</v>
       </c>
-      <c r="J60" s="9">
-        <f t="shared" si="13"/>
+      <c r="J60" s="7">
+        <f t="shared" si="14"/>
         <v>30.8492</v>
       </c>
     </row>
     <row r="61" spans="6:10" x14ac:dyDescent="0.35">
-      <c r="F61" s="8" t="s">
+      <c r="F61" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G61" s="8">
+      <c r="G61" s="6">
         <v>6000</v>
       </c>
-      <c r="H61" s="8">
+      <c r="H61" s="6">
         <v>395000</v>
       </c>
-      <c r="I61" s="8">
+      <c r="I61" s="6">
         <v>75061</v>
       </c>
-      <c r="J61" s="9">
-        <f t="shared" si="13"/>
+      <c r="J61" s="7">
+        <f t="shared" si="14"/>
         <v>10.008133333333333</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="F22:I22"/>
     <mergeCell ref="F57:I57"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="A15:C16"/>
@@ -2065,7 +2108,6 @@
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="A21:C21"/>
-    <mergeCell ref="F22:I22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added the cost breakdown page and adjusted some styling
</commit_message>
<xml_diff>
--- a/cost breakdown.xlsx
+++ b/cost breakdown.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\workspace\java-final-capstone-team7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC3A5493-6F42-444F-9EC9-0528E3CBA463}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A29ED967-2145-4057-B8CD-A3B9A73CAE15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F860004D-61CB-4DE1-A5F2-07380193DBA2}"/>
+    <workbookView xWindow="10830" yWindow="4700" windowWidth="14400" windowHeight="7360" xr2:uid="{F860004D-61CB-4DE1-A5F2-07380193DBA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -248,7 +248,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -259,6 +259,9 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -271,9 +274,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -592,8 +593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B736F933-A202-4884-874F-41D15A360C53}">
   <dimension ref="A1:P61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -624,7 +625,7 @@
       <c r="D1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="11"/>
+      <c r="E1" s="14"/>
       <c r="F1" s="2" t="s">
         <v>22</v>
       </c>
@@ -642,18 +643,18 @@
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="13" t="s">
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
       <c r="J2" s="4"/>
       <c r="L2" t="s">
         <v>46</v>
@@ -685,7 +686,7 @@
         <f>AVERAGE(B3:C3)</f>
         <v>18</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E3" s="10">
         <f>D3/D$17</f>
         <v>0.18045112781954886</v>
       </c>
@@ -739,7 +740,7 @@
         <f t="shared" ref="D4:D14" si="0">AVERAGE(B4:C4)</f>
         <v>2.2000000000000002</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="10">
         <f t="shared" ref="E4:E15" si="1">D4/D$17</f>
         <v>2.2055137844611529E-2</v>
       </c>
@@ -793,7 +794,7 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="10">
         <f t="shared" si="1"/>
         <v>2.0050125313283207E-2</v>
       </c>
@@ -847,7 +848,7 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="10">
         <f t="shared" si="1"/>
         <v>3.007518796992481E-2</v>
       </c>
@@ -901,16 +902,16 @@
         <f t="shared" si="0"/>
         <v>8.5</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="10">
         <f t="shared" si="1"/>
         <v>8.5213032581453629E-2</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
       <c r="L7" t="s">
         <v>48</v>
       </c>
@@ -932,13 +933,13 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
       <c r="D8" s="5"/>
-      <c r="E8" s="14"/>
+      <c r="E8" s="10"/>
       <c r="F8" s="5" t="s">
         <v>23</v>
       </c>
@@ -973,7 +974,7 @@
         <f t="shared" si="0"/>
         <v>9.4</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E9" s="10">
         <f t="shared" si="1"/>
         <v>9.4235588972431075E-2</v>
       </c>
@@ -1021,7 +1022,7 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E10" s="14">
+      <c r="E10" s="10">
         <f t="shared" si="1"/>
         <v>3.007518796992481E-2</v>
       </c>
@@ -1070,7 +1071,7 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11" s="10">
         <f t="shared" si="1"/>
         <v>3.007518796992481E-2</v>
       </c>
@@ -1119,16 +1120,16 @@
         <f t="shared" si="0"/>
         <v>2.25</v>
       </c>
-      <c r="E12" s="14">
+      <c r="E12" s="10">
         <f t="shared" si="1"/>
         <v>2.2556390977443608E-2</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F12" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
       <c r="L12" t="s">
         <v>25</v>
       </c>
@@ -1158,7 +1159,7 @@
         <f t="shared" si="0"/>
         <v>3.4000000000000004</v>
       </c>
-      <c r="E13" s="14">
+      <c r="E13" s="10">
         <f t="shared" si="1"/>
         <v>3.4085213032581455E-2</v>
       </c>
@@ -1207,7 +1208,7 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="E14" s="14">
+      <c r="E14" s="10">
         <f t="shared" si="1"/>
         <v>0.15037593984962405</v>
       </c>
@@ -1240,15 +1241,15 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
       <c r="D15" s="5">
         <v>30</v>
       </c>
-      <c r="E15" s="14">
+      <c r="E15" s="10">
         <f t="shared" si="1"/>
         <v>0.3007518796992481</v>
       </c>
@@ -1281,10 +1282,10 @@
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="E16" s="15"/>
+      <c r="A16" s="15"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="E16" s="11"/>
       <c r="F16" s="6" t="s">
         <v>26</v>
       </c>
@@ -1306,19 +1307,24 @@
       <c r="C17" t="s">
         <v>47</v>
       </c>
-      <c r="D17" s="16">
+      <c r="D17" s="12">
         <f>SUM(D3:D15)</f>
         <v>99.75</v>
       </c>
-      <c r="E17" s="7"/>
-      <c r="F17" s="10" t="s">
+      <c r="E17" s="17">
+        <v>89.78</v>
+      </c>
+      <c r="F17" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="E18" s="17">
+        <v>109.73</v>
+      </c>
       <c r="F18" s="5" t="s">
         <v>23</v>
       </c>
@@ -1373,11 +1379,11 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
       <c r="D21" s="5"/>
       <c r="F21" s="6" t="s">
         <v>26</v>
@@ -1410,12 +1416,12 @@
         <f>AVERAGE(B22:C22)</f>
         <v>51625</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="F22" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
@@ -1530,12 +1536,12 @@
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="F27" s="10" t="s">
+      <c r="F27" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="F28" s="5" t="s">
@@ -1610,12 +1616,12 @@
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="F32" s="10" t="s">
+      <c r="F32" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="G32" s="10"/>
-      <c r="H32" s="10"/>
-      <c r="I32" s="10"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="13"/>
     </row>
     <row r="33" spans="6:10" x14ac:dyDescent="0.35">
       <c r="F33" s="5" t="s">
@@ -1690,12 +1696,12 @@
       </c>
     </row>
     <row r="37" spans="6:10" x14ac:dyDescent="0.35">
-      <c r="F37" s="10" t="s">
+      <c r="F37" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="G37" s="10"/>
-      <c r="H37" s="10"/>
-      <c r="I37" s="10"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="13"/>
     </row>
     <row r="38" spans="6:10" x14ac:dyDescent="0.35">
       <c r="F38" s="5" t="s">
@@ -1770,12 +1776,12 @@
       </c>
     </row>
     <row r="42" spans="6:10" x14ac:dyDescent="0.35">
-      <c r="F42" s="10" t="s">
+      <c r="F42" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="G42" s="10"/>
-      <c r="H42" s="10"/>
-      <c r="I42" s="10"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="13"/>
+      <c r="I42" s="13"/>
     </row>
     <row r="43" spans="6:10" x14ac:dyDescent="0.35">
       <c r="F43" s="5" t="s">
@@ -1850,12 +1856,12 @@
       </c>
     </row>
     <row r="47" spans="6:10" x14ac:dyDescent="0.35">
-      <c r="F47" s="10" t="s">
+      <c r="F47" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="G47" s="10"/>
-      <c r="H47" s="10"/>
-      <c r="I47" s="10"/>
+      <c r="G47" s="13"/>
+      <c r="H47" s="13"/>
+      <c r="I47" s="13"/>
     </row>
     <row r="48" spans="6:10" x14ac:dyDescent="0.35">
       <c r="F48" s="5" t="s">
@@ -1930,12 +1936,12 @@
       </c>
     </row>
     <row r="52" spans="6:10" x14ac:dyDescent="0.35">
-      <c r="F52" s="10" t="s">
+      <c r="F52" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="G52" s="10"/>
-      <c r="H52" s="10"/>
-      <c r="I52" s="10"/>
+      <c r="G52" s="13"/>
+      <c r="H52" s="13"/>
+      <c r="I52" s="13"/>
     </row>
     <row r="53" spans="6:10" x14ac:dyDescent="0.35">
       <c r="F53" s="5" t="s">
@@ -2010,12 +2016,12 @@
       </c>
     </row>
     <row r="57" spans="6:10" x14ac:dyDescent="0.35">
-      <c r="F57" s="10" t="s">
+      <c r="F57" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="G57" s="10"/>
-      <c r="H57" s="10"/>
-      <c r="I57" s="10"/>
+      <c r="G57" s="13"/>
+      <c r="H57" s="13"/>
+      <c r="I57" s="13"/>
     </row>
     <row r="58" spans="6:10" x14ac:dyDescent="0.35">
       <c r="F58" s="5" t="s">
@@ -2091,6 +2097,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A21:C21"/>
     <mergeCell ref="F22:I22"/>
     <mergeCell ref="F57:I57"/>
     <mergeCell ref="E1:E2"/>
@@ -2107,7 +2114,6 @@
     <mergeCell ref="F17:I17"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A21:C21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>